<commit_message>
Upgraded to product sheet with enter amounts by product. Also fixed issue for customer not found due to forwarding change made
</commit_message>
<xml_diff>
--- a/AutoBlueSystemSrc/customer_product_codes/orders@choco.app_DANTER.xlsx
+++ b/AutoBlueSystemSrc/customer_product_codes/orders@choco.app_DANTER.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,7 +431,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>2 32BUCA 5E</t>
+          <t>2 32BUCA</t>
         </is>
       </c>
     </row>
@@ -445,7 +445,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2 P1LING 4E</t>
+          <t>2 P1LING</t>
         </is>
       </c>
     </row>
@@ -459,7 +459,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4 P1PAPP 4E</t>
+          <t>4 P1PAPP</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,21 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2 P1PAPP 4E</t>
+          <t>2 P1PAPP</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>bucatini
+case
+1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1 32BUCA</t>
         </is>
       </c>
     </row>

</xml_diff>